<commit_message>
Add interpolation rule for ACT_BND
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_No_Bound.xlsx
+++ b/SuppXLS/Scen_TRA_No_Bound.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FE7AA6-B177-419F-8D19-AFAE77CCE0DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF4E90C-81C3-4EF3-8926-03694D0DF360}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -723,7 +723,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFC0D1CC-CDCE-448C-AFA9-77FF370A76F3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000010C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -780,8 +780,8 @@
       <sheetName val="On-Road Fac."/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="11">
@@ -915,15 +915,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2131,6 +2131,9 @@
       <c r="E8">
         <v>0</v>
       </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
       <c r="J8" t="str">
         <f>J7</f>
         <v>FT-TRAETH</v>
@@ -2158,6 +2161,9 @@
       </c>
       <c r="E10">
         <v>0</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
       </c>
       <c r="J10" s="15" t="str">
         <f>J9</f>

</xml_diff>